<commit_message>
pushing latest status. Transform app and its output added
</commit_message>
<xml_diff>
--- a/ClineG_TimeCard.xlsx
+++ b/ClineG_TimeCard.xlsx
@@ -382,7 +382,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,9 +429,12 @@
       <c r="F2">
         <v>5.5</v>
       </c>
+      <c r="G2">
+        <v>4.5</v>
+      </c>
       <c r="I2">
         <f>SUM(B2:H2)</f>
-        <v>13.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -480,7 +483,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
@@ -488,7 +491,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>13.5</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>